<commit_message>
From v1.2.5 to v1.3
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Solicitar Diárias--GT-.xlsx
+++ b/output/xlsx/UC001 - Solicitar Diárias--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="81">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Version: </t>
   </si>
   <si>
-    <t>1.2.5</t>
+    <t>1.3</t>
   </si>
   <si>
     <t>Suite Type:</t>
@@ -92,6 +92,132 @@
     <t>Actual Result</t>
   </si>
   <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem nacional - dentro do estado (intermunicipal).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opção escolhida: viagem nacional - dentro do estado (intermunicipal).</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário NÃO Escolhe o estado.</t>
+  </si>
+  <si>
+    <t>SYSTEM O sistema seleciona o estado como PB, automaticamente.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe a(s) cidade(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opção escolhida: cidade(s).</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de deslocamento.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opção escolhida: tipo de deslocamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de hospedagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opção escolhida: hospedagem.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de período de afastamento.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opção escolhida: período de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, após o último dia de viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opção escolhida: pernoite.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opção escolhida: justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Detalha a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o(s) beneficiário(s) da(s) diária(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe os beneficiário(s) selecionado(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Confirma a existência de conta para recebimento de diárias do servidor.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em confirmar.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe uma mensagem de alerta informando sobre o estouro do limite de 10 diárias por mês.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Fecha o alerta</t>
+  </si>
+  <si>
+    <t>SYSTEM Calcula o valor da(s) diária(s) com as informações do formulário.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de uma diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado. 3. Manutenção do cargo comissionado e do setor beneficiário à época da concessão da diária.</t>
+  </si>
+  <si>
+    <t>SYSTEM Altera o status da diária para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>O sistema salva os dados.</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opção escolhida: país da viagem.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do último dia de viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe os beneficiário(s) selecionado(s) e o campo para preenchimento do nome social.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa o nome social do beneficiário da(s) diária(s).</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em limpar campos.</t>
+  </si>
+  <si>
+    <t>SYSTEM Apaga todas as seleções do usuário.</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
     <t>Chefe/Beneficiário Escolhe o tipo de viagem nacional - fora do estado (interestadual).</t>
   </si>
   <si>
@@ -104,139 +230,19 @@
     <t>SYSTEM Exibe a opção escolhida: estado.</t>
   </si>
   <si>
-    <t>Chefe/Beneficiário Escolhe a(s) cidade(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opção escolhida: cidade(s).</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de deslocamento.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opção escolhida: tipo de deslocamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de hospedagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opção escolhida: hospedagem.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de período de afastamento.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opção escolhida: período de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do último dia de viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opção escolhida: pernoite.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opção escolhida: justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Detalha a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o(s) beneficiário(s) da(s) diária(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe os beneficiário(s) selecionado(s) e o campo para preenchimento do nome social.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa o nome social do beneficiário da(s) diária(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Confirma a existência de conta para recebimento de diárias do servidor.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em confirmar.</t>
-  </si>
-  <si>
-    <t>SYSTEM Calcula o valor da(s) diária(s) com as informações do formulário.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de uma diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado. 3. Manutenção do cargo comissionado e do setor beneficiário à época da concessão da diária.</t>
-  </si>
-  <si>
-    <t>SYSTEM Altera o status da diária para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>O sistema salva os dados.</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opção escolhida: país da viagem.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, após o último dia de viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe os beneficiário(s) selecionado(s).</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em limpar campos.</t>
-  </si>
-  <si>
-    <t>SYSTEM Apaga todas as seleções do usuário.</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem nacional - dentro do estado (intermunicipal).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opção escolhida: viagem nacional - dentro do estado (intermunicipal).</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário NÃO Escolhe o estado.</t>
-  </si>
-  <si>
-    <t>SYSTEM O sistema seleciona o estado como PB, automaticamente.</t>
+    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
+  </si>
+  <si>
+    <t>TC5</t>
   </si>
   <si>
     <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
-  </si>
-  <si>
-    <t>TC4</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
-  </si>
-  <si>
-    <t>TC5</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
   </si>
   <si>
     <t>TC6</t>
@@ -444,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F123"/>
+  <dimension ref="A1:F124"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -825,13 +831,13 @@
         <v>12.0</v>
       </c>
       <c r="B21" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s" s="7">
         <v>48</v>
-      </c>
-      <c r="C21" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s" s="7">
-        <v>49</v>
       </c>
       <c r="E21" t="s" s="6">
         <v>2</v>
@@ -845,13 +851,13 @@
         <v>13.0</v>
       </c>
       <c r="B22" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s" s="7">
         <v>50</v>
-      </c>
-      <c r="C22" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s" s="7">
-        <v>51</v>
       </c>
       <c r="E22" t="s" s="6">
         <v>2</v>
@@ -865,155 +871,155 @@
         <v>14.0</v>
       </c>
       <c r="B23" t="s" s="7">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s" s="7">
         <v>52</v>
       </c>
-      <c r="C23" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s" s="7">
+      <c r="E23" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n" s="10">
+        <v>15.0</v>
+      </c>
+      <c r="B24" t="s" s="7">
         <v>53</v>
       </c>
-      <c r="E23" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F23" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="8">
+      <c r="C24" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s" s="7">
         <v>54</v>
       </c>
-      <c r="B24" t="s" s="8">
+      <c r="E24" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="8">
         <v>55</v>
       </c>
-      <c r="C24" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F24" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25"/>
+      <c r="B25" t="s" s="8">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
     <row r="26"/>
-    <row r="27">
-      <c r="A27" t="s" s="4">
+    <row r="27"/>
+    <row r="28">
+      <c r="A28" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B27" t="s" s="4">
-        <v>56</v>
-      </c>
-      <c r="C27" t="s" s="4">
+      <c r="B28" t="s" s="4">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D27" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E27" t="s" s="4">
+      <c r="D28" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F27" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="9">
+      <c r="F28" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B28" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E28" t="s" s="9">
+      <c r="B29" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F28" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="8">
+      <c r="F29" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B29" t="s" s="8">
+      <c r="B30" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C29" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E29" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F29" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="5">
+      <c r="C30" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B30" t="s" s="5">
+      <c r="B31" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C30" t="s" s="5">
+      <c r="C31" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D30" t="s" s="5">
+      <c r="D31" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E30" t="s" s="5">
+      <c r="E31" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F30" t="s" s="5">
+      <c r="F31" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B31" t="s" s="7">
-        <v>57</v>
-      </c>
-      <c r="C31" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s" s="7">
-        <v>58</v>
-      </c>
-      <c r="E31" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F31" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B32" t="s" s="7">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s" s="7">
         <v>59</v>
-      </c>
-      <c r="C32" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s" s="7">
-        <v>60</v>
       </c>
       <c r="E32" t="s" s="6">
         <v>2</v>
@@ -1024,16 +1030,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n" s="10">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B33" t="s" s="7">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D33" t="s" s="7">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="E33" t="s" s="6">
         <v>2</v>
@@ -1044,16 +1050,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n" s="10">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B34" t="s" s="7">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C34" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D34" t="s" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E34" t="s" s="6">
         <v>2</v>
@@ -1064,16 +1070,16 @@
     </row>
     <row r="35">
       <c r="A35" t="n" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B35" t="s" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D35" t="s" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E35" t="s" s="6">
         <v>2</v>
@@ -1084,16 +1090,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n" s="10">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B36" t="s" s="7">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D36" t="s" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E36" t="s" s="6">
         <v>2</v>
@@ -1104,16 +1110,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n" s="10">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B37" t="s" s="7">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D37" t="s" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E37" t="s" s="6">
         <v>2</v>
@@ -1124,16 +1130,16 @@
     </row>
     <row r="38">
       <c r="A38" t="n" s="10">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B38" t="s" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D38" t="s" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E38" t="s" s="6">
         <v>2</v>
@@ -1144,16 +1150,16 @@
     </row>
     <row r="39">
       <c r="A39" t="n" s="10">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B39" t="s" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D39" t="s" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E39" t="s" s="6">
         <v>2</v>
@@ -1164,16 +1170,16 @@
     </row>
     <row r="40">
       <c r="A40" t="n" s="10">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B40" t="s" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D40" t="s" s="7">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E40" t="s" s="6">
         <v>2</v>
@@ -1184,7 +1190,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n" s="10">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B41" t="s" s="7">
         <v>46</v>
@@ -1193,7 +1199,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s" s="7">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E41" t="s" s="6">
         <v>2</v>
@@ -1204,129 +1210,129 @@
     </row>
     <row r="42">
       <c r="A42" t="n" s="10">
+        <v>11.0</v>
+      </c>
+      <c r="B42" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="C42" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="E42" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n" s="10">
         <v>12.0</v>
       </c>
-      <c r="B42" t="s" s="7">
-        <v>63</v>
-      </c>
-      <c r="C42" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s" s="7">
-        <v>64</v>
-      </c>
-      <c r="E42" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F42" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43"/>
+      <c r="B43" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="C43" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="44"/>
-    <row r="45">
-      <c r="A45" t="s" s="4">
+    <row r="45"/>
+    <row r="46">
+      <c r="A46" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B45" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="C45" t="s" s="4">
+      <c r="B46" t="s" s="4">
+        <v>67</v>
+      </c>
+      <c r="C46" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D45" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E45" t="s" s="4">
+      <c r="D46" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F45" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s" s="9">
+      <c r="F46" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B46" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C46" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E46" t="s" s="9">
+      <c r="B47" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F46" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s" s="8">
+      <c r="F47" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B47" t="s" s="8">
+      <c r="B48" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C47" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D47" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E47" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F47" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="5">
+      <c r="C48" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B48" t="s" s="5">
+      <c r="B49" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C48" t="s" s="5">
+      <c r="C49" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D48" t="s" s="5">
+      <c r="D49" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E48" t="s" s="5">
+      <c r="E49" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F48" t="s" s="5">
+      <c r="F49" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B49" t="s" s="7">
-        <v>66</v>
-      </c>
-      <c r="C49" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D49" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="E49" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F49" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B50" t="s" s="7">
         <v>68</v>
@@ -1346,16 +1352,16 @@
     </row>
     <row r="51">
       <c r="A51" t="n" s="10">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B51" t="s" s="7">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D51" t="s" s="7">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="E51" t="s" s="6">
         <v>2</v>
@@ -1366,16 +1372,16 @@
     </row>
     <row r="52">
       <c r="A52" t="n" s="10">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B52" t="s" s="7">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D52" t="s" s="7">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E52" t="s" s="6">
         <v>2</v>
@@ -1386,16 +1392,16 @@
     </row>
     <row r="53">
       <c r="A53" t="n" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B53" t="s" s="7">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C53" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D53" t="s" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E53" t="s" s="6">
         <v>2</v>
@@ -1406,16 +1412,16 @@
     </row>
     <row r="54">
       <c r="A54" t="n" s="10">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B54" t="s" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C54" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D54" t="s" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E54" t="s" s="6">
         <v>2</v>
@@ -1426,16 +1432,16 @@
     </row>
     <row r="55">
       <c r="A55" t="n" s="10">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B55" t="s" s="7">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="C55" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D55" t="s" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E55" t="s" s="6">
         <v>2</v>
@@ -1446,16 +1452,16 @@
     </row>
     <row r="56">
       <c r="A56" t="n" s="10">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B56" t="s" s="7">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C56" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D56" t="s" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E56" t="s" s="6">
         <v>2</v>
@@ -1466,16 +1472,16 @@
     </row>
     <row r="57">
       <c r="A57" t="n" s="10">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B57" t="s" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C57" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D57" t="s" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E57" t="s" s="6">
         <v>2</v>
@@ -1486,16 +1492,16 @@
     </row>
     <row r="58">
       <c r="A58" t="n" s="10">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B58" t="s" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C58" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D58" t="s" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E58" t="s" s="6">
         <v>2</v>
@@ -1506,16 +1512,16 @@
     </row>
     <row r="59">
       <c r="A59" t="n" s="10">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B59" t="s" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C59" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D59" t="s" s="7">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E59" t="s" s="6">
         <v>2</v>
@@ -1526,7 +1532,7 @@
     </row>
     <row r="60">
       <c r="A60" t="n" s="10">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="B60" t="s" s="7">
         <v>46</v>
@@ -1535,7 +1541,7 @@
         <v>2</v>
       </c>
       <c r="D60" t="s" s="7">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E60" t="s" s="6">
         <v>2</v>
@@ -1544,140 +1550,140 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63">
-      <c r="A63" t="s" s="4">
+    <row r="61">
+      <c r="A61" t="n" s="10">
+        <v>12.0</v>
+      </c>
+      <c r="B61" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="C61" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="E61" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F61" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n" s="10">
+        <v>13.0</v>
+      </c>
+      <c r="B62" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="C62" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="E62" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F62" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65">
+      <c r="A65" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B63" t="s" s="4">
-        <v>71</v>
-      </c>
-      <c r="C63" t="s" s="4">
+      <c r="B65" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="C65" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D63" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E63" t="s" s="4">
+      <c r="D65" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F63" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s" s="9">
+      <c r="F65" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s" s="9">
+      <c r="B66" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F64" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="8">
+      <c r="F66" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B65" t="s" s="8">
+      <c r="B67" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F65" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s" s="5">
+      <c r="C67" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E67" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F67" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B66" t="s" s="5">
+      <c r="B68" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C66" t="s" s="5">
+      <c r="C68" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D66" t="s" s="5">
+      <c r="D68" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E66" t="s" s="5">
+      <c r="E68" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F66" t="s" s="5">
+      <c r="F68" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B67" t="s" s="7">
-        <v>66</v>
-      </c>
-      <c r="C67" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D67" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="E67" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F67" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B68" t="s" s="7">
-        <v>68</v>
-      </c>
-      <c r="C68" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D68" t="s" s="7">
-        <v>69</v>
-      </c>
-      <c r="E68" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F68" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n" s="10">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B69" t="s" s="7">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C69" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E69" t="s" s="6">
         <v>2</v>
@@ -1688,16 +1694,16 @@
     </row>
     <row r="70">
       <c r="A70" t="n" s="10">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="B70" t="s" s="7">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C70" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D70" t="s" s="7">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E70" t="s" s="6">
         <v>2</v>
@@ -1708,16 +1714,16 @@
     </row>
     <row r="71">
       <c r="A71" t="n" s="10">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="B71" t="s" s="7">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C71" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D71" t="s" s="7">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E71" t="s" s="6">
         <v>2</v>
@@ -1728,16 +1734,16 @@
     </row>
     <row r="72">
       <c r="A72" t="n" s="10">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="B72" t="s" s="7">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C72" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D72" t="s" s="7">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E72" t="s" s="6">
         <v>2</v>
@@ -1748,16 +1754,16 @@
     </row>
     <row r="73">
       <c r="A73" t="n" s="10">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="B73" t="s" s="7">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C73" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D73" t="s" s="7">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E73" t="s" s="6">
         <v>2</v>
@@ -1768,16 +1774,16 @@
     </row>
     <row r="74">
       <c r="A74" t="n" s="10">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="B74" t="s" s="7">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C74" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D74" t="s" s="7">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E74" t="s" s="6">
         <v>2</v>
@@ -1788,16 +1794,16 @@
     </row>
     <row r="75">
       <c r="A75" t="n" s="10">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
       <c r="B75" t="s" s="7">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C75" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D75" t="s" s="7">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E75" t="s" s="6">
         <v>2</v>
@@ -1808,16 +1814,16 @@
     </row>
     <row r="76">
       <c r="A76" t="n" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="B76" t="s" s="7">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C76" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D76" t="s" s="7">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E76" t="s" s="6">
         <v>2</v>
@@ -1828,16 +1834,16 @@
     </row>
     <row r="77">
       <c r="A77" t="n" s="10">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="B77" t="s" s="7">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C77" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D77" t="s" s="7">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E77" t="s" s="6">
         <v>2</v>
@@ -1848,16 +1854,16 @@
     </row>
     <row r="78">
       <c r="A78" t="n" s="10">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="B78" t="s" s="7">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C78" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D78" t="s" s="7">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E78" t="s" s="6">
         <v>2</v>
@@ -1868,178 +1874,178 @@
     </row>
     <row r="79">
       <c r="A79" t="n" s="10">
+        <v>11.0</v>
+      </c>
+      <c r="B79" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C79" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="E79" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F79" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n" s="10">
+        <v>12.0</v>
+      </c>
+      <c r="B80" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="C80" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="E80" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F80" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n" s="10">
         <v>13.0</v>
       </c>
-      <c r="B79" t="s" s="7">
+      <c r="B81" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="C81" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s" s="7">
         <v>50</v>
       </c>
-      <c r="C79" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D79" t="s" s="7">
-        <v>72</v>
-      </c>
-      <c r="E79" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F79" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80"/>
-    <row r="81"/>
+      <c r="E81" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F81" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="82">
-      <c r="A82" t="s" s="4">
+      <c r="A82" t="n" s="10">
+        <v>14.0</v>
+      </c>
+      <c r="B82" t="s" s="7">
+        <v>51</v>
+      </c>
+      <c r="C82" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="E82" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F82" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85">
+      <c r="A85" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B82" t="s" s="4">
-        <v>73</v>
-      </c>
-      <c r="C82" t="s" s="4">
+      <c r="B85" t="s" s="4">
+        <v>75</v>
+      </c>
+      <c r="C85" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D82" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E82" t="s" s="4">
+      <c r="D85" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E85" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F82" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s" s="9">
+      <c r="F85" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E83" t="s" s="9">
+      <c r="B86" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C86" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D86" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E86" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F83" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s" s="8">
+      <c r="F86" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B84" t="s" s="8">
+      <c r="B87" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F84" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s" s="5">
+      <c r="C87" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D87" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E87" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F87" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B85" t="s" s="5">
+      <c r="B88" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C85" t="s" s="5">
+      <c r="C88" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D85" t="s" s="5">
+      <c r="D88" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E85" t="s" s="5">
+      <c r="E88" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F85" t="s" s="5">
+      <c r="F88" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B86" t="s" s="7">
-        <v>66</v>
-      </c>
-      <c r="C86" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D86" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="E86" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F86" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B87" t="s" s="7">
-        <v>68</v>
-      </c>
-      <c r="C87" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D87" t="s" s="7">
-        <v>69</v>
-      </c>
-      <c r="E87" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F87" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="B88" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="C88" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D88" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="E88" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F88" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n" s="10">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="B89" t="s" s="7">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C89" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D89" t="s" s="7">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="E89" t="s" s="6">
         <v>2</v>
@@ -2050,16 +2056,16 @@
     </row>
     <row r="90">
       <c r="A90" t="n" s="10">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="B90" t="s" s="7">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C90" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D90" t="s" s="7">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="E90" t="s" s="6">
         <v>2</v>
@@ -2070,16 +2076,16 @@
     </row>
     <row r="91">
       <c r="A91" t="n" s="10">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="B91" t="s" s="7">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C91" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D91" t="s" s="7">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E91" t="s" s="6">
         <v>2</v>
@@ -2090,16 +2096,16 @@
     </row>
     <row r="92">
       <c r="A92" t="n" s="10">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="B92" t="s" s="7">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C92" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D92" t="s" s="7">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E92" t="s" s="6">
         <v>2</v>
@@ -2110,16 +2116,16 @@
     </row>
     <row r="93">
       <c r="A93" t="n" s="10">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="B93" t="s" s="7">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C93" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D93" t="s" s="7">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E93" t="s" s="6">
         <v>2</v>
@@ -2130,16 +2136,16 @@
     </row>
     <row r="94">
       <c r="A94" t="n" s="10">
-        <v>9.0</v>
+        <v>6.0</v>
       </c>
       <c r="B94" t="s" s="7">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C94" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D94" t="s" s="7">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E94" t="s" s="6">
         <v>2</v>
@@ -2150,16 +2156,16 @@
     </row>
     <row r="95">
       <c r="A95" t="n" s="10">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
       <c r="B95" t="s" s="7">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C95" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D95" t="s" s="7">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E95" t="s" s="6">
         <v>2</v>
@@ -2170,16 +2176,16 @@
     </row>
     <row r="96">
       <c r="A96" t="n" s="10">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="B96" t="s" s="7">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C96" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D96" t="s" s="7">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E96" t="s" s="6">
         <v>2</v>
@@ -2190,16 +2196,16 @@
     </row>
     <row r="97">
       <c r="A97" t="n" s="10">
-        <v>12.0</v>
+        <v>9.0</v>
       </c>
       <c r="B97" t="s" s="7">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C97" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D97" t="s" s="7">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E97" t="s" s="6">
         <v>2</v>
@@ -2210,16 +2216,16 @@
     </row>
     <row r="98">
       <c r="A98" t="n" s="10">
-        <v>13.0</v>
+        <v>10.0</v>
       </c>
       <c r="B98" t="s" s="7">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C98" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D98" t="s" s="7">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E98" t="s" s="6">
         <v>2</v>
@@ -2228,120 +2234,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99"/>
+    <row r="99">
+      <c r="A99" t="n" s="10">
+        <v>11.0</v>
+      </c>
+      <c r="B99" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="C99" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="E99" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F99" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="100"/>
-    <row r="101">
-      <c r="A101" t="s" s="4">
+    <row r="101"/>
+    <row r="102">
+      <c r="A102" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B101" t="s" s="4">
-        <v>75</v>
-      </c>
-      <c r="C101" t="s" s="4">
+      <c r="B102" t="s" s="4">
+        <v>77</v>
+      </c>
+      <c r="C102" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D101" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E101" t="s" s="4">
+      <c r="D102" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E102" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F101" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s" s="9">
+      <c r="F102" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B102" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C102" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D102" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E102" t="s" s="9">
+      <c r="B103" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E103" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F102" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s" s="8">
+      <c r="F103" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B103" t="s" s="8">
+      <c r="B104" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C103" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D103" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E103" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F103" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s" s="5">
+      <c r="C104" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D104" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E104" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F104" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B104" t="s" s="5">
+      <c r="B105" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C104" t="s" s="5">
+      <c r="C105" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D104" t="s" s="5">
+      <c r="D105" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E104" t="s" s="5">
+      <c r="E105" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F104" t="s" s="5">
+      <c r="F105" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B105" t="s" s="7">
-        <v>66</v>
-      </c>
-      <c r="C105" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D105" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="E105" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F105" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B106" t="s" s="7">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="C106" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D106" t="s" s="7">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="E106" t="s" s="6">
         <v>2</v>
@@ -2352,16 +2358,16 @@
     </row>
     <row r="107">
       <c r="A107" t="n" s="10">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B107" t="s" s="7">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C107" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D107" t="s" s="7">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E107" t="s" s="6">
         <v>2</v>
@@ -2372,16 +2378,16 @@
     </row>
     <row r="108">
       <c r="A108" t="n" s="10">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B108" t="s" s="7">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C108" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D108" t="s" s="7">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E108" t="s" s="6">
         <v>2</v>
@@ -2392,16 +2398,16 @@
     </row>
     <row r="109">
       <c r="A109" t="n" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B109" t="s" s="7">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C109" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D109" t="s" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E109" t="s" s="6">
         <v>2</v>
@@ -2412,16 +2418,16 @@
     </row>
     <row r="110">
       <c r="A110" t="n" s="10">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B110" t="s" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C110" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D110" t="s" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E110" t="s" s="6">
         <v>2</v>
@@ -2432,16 +2438,16 @@
     </row>
     <row r="111">
       <c r="A111" t="n" s="10">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B111" t="s" s="7">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="C111" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D111" t="s" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E111" t="s" s="6">
         <v>2</v>
@@ -2452,16 +2458,16 @@
     </row>
     <row r="112">
       <c r="A112" t="n" s="10">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B112" t="s" s="7">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C112" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D112" t="s" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E112" t="s" s="6">
         <v>2</v>
@@ -2472,16 +2478,16 @@
     </row>
     <row r="113">
       <c r="A113" t="n" s="10">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B113" t="s" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C113" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D113" t="s" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E113" t="s" s="6">
         <v>2</v>
@@ -2492,16 +2498,16 @@
     </row>
     <row r="114">
       <c r="A114" t="n" s="10">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B114" t="s" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C114" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D114" t="s" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E114" t="s" s="6">
         <v>2</v>
@@ -2512,143 +2518,163 @@
     </row>
     <row r="115">
       <c r="A115" t="n" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="B115" t="s" s="7">
+        <v>44</v>
+      </c>
+      <c r="C115" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D115" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="E115" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F115" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n" s="10">
         <v>11.0</v>
       </c>
-      <c r="B115" t="s" s="7">
+      <c r="B116" t="s" s="7">
         <v>46</v>
       </c>
-      <c r="C115" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D115" t="s" s="7">
-        <v>76</v>
-      </c>
-      <c r="E115" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F115" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="116"/>
+      <c r="C116" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D116" t="s" s="7">
+        <v>78</v>
+      </c>
+      <c r="E116" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F116" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="117"/>
-    <row r="118">
-      <c r="A118" t="s" s="4">
+    <row r="118"/>
+    <row r="119">
+      <c r="A119" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B118" t="s" s="4">
-        <v>77</v>
-      </c>
-      <c r="C118" t="s" s="4">
+      <c r="B119" t="s" s="4">
+        <v>79</v>
+      </c>
+      <c r="C119" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D118" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E118" t="s" s="4">
+      <c r="D119" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E119" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F118" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="s" s="9">
+      <c r="F119" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B119" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C119" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D119" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E119" t="s" s="9">
+      <c r="B120" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C120" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D120" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E120" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F119" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="s" s="8">
+      <c r="F120" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B120" t="s" s="8">
+      <c r="B121" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C120" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D120" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E120" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F120" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="s" s="5">
+      <c r="C121" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D121" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E121" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F121" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B121" t="s" s="5">
+      <c r="B122" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C121" t="s" s="5">
+      <c r="C122" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D121" t="s" s="5">
+      <c r="D122" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E121" t="s" s="5">
+      <c r="E122" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F121" t="s" s="5">
+      <c r="F122" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B122" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="C122" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D122" t="s" s="7">
-        <v>27</v>
-      </c>
-      <c r="E122" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F122" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B123" t="s" s="7">
+        <v>68</v>
+      </c>
+      <c r="C123" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D123" t="s" s="7">
+        <v>69</v>
+      </c>
+      <c r="E123" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F123" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n" s="10">
         <v>2.0</v>
       </c>
-      <c r="B123" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="C123" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D123" t="s" s="7">
-        <v>78</v>
-      </c>
-      <c r="E123" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F123" t="s" s="6">
+      <c r="B124" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="C124" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D124" t="s" s="7">
+        <v>80</v>
+      </c>
+      <c r="E124" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F124" t="s" s="6">
         <v>2</v>
       </c>
     </row>
@@ -2657,19 +2683,19 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B120:D120"/>
+    <mergeCell ref="B121:F121"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>